<commit_message>
Name of generated file edite
</commit_message>
<xml_diff>
--- a/Input_Data.xlsx
+++ b/Input_Data.xlsx
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:19.634373</t>
+          <t>2022-03-15 15:01:56.185909</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:21.819795</t>
+          <t>2022-03-15 15:01:57.107958</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:23.167885</t>
+          <t>2022-03-15 15:01:58.700224</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:27.693122</t>
+          <t>2022-03-15 15:02:01.189186</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
@@ -503,11 +503,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:29.847724</t>
+          <t>2022-03-15 15:02:02.684583</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:31.289940</t>
+          <t>2022-03-15 15:02:03.720169</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:32.628274</t>
+          <t>2022-03-15 15:02:04.413693</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9">
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:33.609967</t>
+          <t>2022-03-15 15:02:06.472708</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:35.052151</t>
+          <t>2022-03-15 15:02:07.204546</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:36.099290</t>
+          <t>2022-03-15 15:02:07.953563</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:37.989103</t>
+          <t>2022-03-15 15:02:08.667783</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:38.785313</t>
+          <t>2022-03-15 15:02:09.492311</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:41.171867</t>
+          <t>2022-03-15 15:02:10.457625</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:42.247340</t>
+          <t>2022-03-15 15:02:11.600791</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:43.635119</t>
+          <t>2022-03-15 15:02:12.681954</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:45.570972</t>
+          <t>2022-03-15 15:02:13.545104</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:47.282242</t>
+          <t>2022-03-15 15:02:14.608945</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:48.053963</t>
+          <t>2022-03-15 15:02:15.523652</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:48.759652</t>
+          <t>2022-03-15 15:02:16.385645</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:49.474610</t>
+          <t>2022-03-15 15:02:16.842992</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2022-03-15 14:53:50.196225</t>
+          <t>2022-03-15 15:02:17.298025</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>